<commit_message>
Minor Modified til UserRegion with different users
</commit_message>
<xml_diff>
--- a/Lexis-GLOBAL/Coredata/REGION.xlsx
+++ b/Lexis-GLOBAL/Coredata/REGION.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adapp\git\AutoAPI\Lexis-GLOBAL\Coredata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341C9C8A-EBA8-44EB-A670-D1A6E25B59F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B0E379-D938-464E-BCB3-C6DC37FFB3EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Region_Create" sheetId="7" r:id="rId1"/>
@@ -669,7 +669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F83A6FB-A034-4DD8-86B8-CFDDCA5856F5}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -1118,7 +1118,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BCC0056-177B-49CB-8A80-CE2D5DAC6381}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="S3" sqref="S3:S7"/>
     </sheetView>
   </sheetViews>

</xml_diff>